<commit_message>
corrected 1770 to 1779
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_0779.xlsx
+++ b/bioSample/bioSample_0779.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417C3D9D-223C-0347-865E-26B03C7CAAFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27B13F3-5330-214E-86CA-61FC0DD12EC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>37C.CO2</t>
   </si>
   <si>
-    <t>TDY1770</t>
-  </si>
-  <si>
     <t>CNAG_04864.CNAG_05420</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>TDY451</t>
+  </si>
+  <si>
+    <t>TDY1779</t>
   </si>
 </sst>
 </file>
@@ -485,13 +485,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1022" width="8.83203125" customWidth="1"/>
+    <col min="1" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" customWidth="1"/>
+    <col min="7" max="1022" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -537,7 +539,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -566,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -595,7 +597,7 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -624,10 +626,10 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -653,10 +655,10 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
@@ -682,10 +684,10 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -711,10 +713,10 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
@@ -740,10 +742,10 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
         <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
@@ -769,10 +771,10 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
         <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
@@ -798,10 +800,10 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>
@@ -827,10 +829,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
         <v>13</v>
@@ -844,7 +846,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -856,7 +858,7 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
@@ -873,7 +875,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -885,7 +887,7 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
@@ -902,7 +904,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -914,7 +916,7 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -931,7 +933,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -943,10 +945,10 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
         <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
@@ -960,7 +962,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -972,10 +974,10 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
         <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>13</v>
@@ -989,7 +991,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -1001,10 +1003,10 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
         <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>21</v>
       </c>
       <c r="G18" t="s">
         <v>13</v>
@@ -1018,7 +1020,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -1030,10 +1032,10 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
         <v>22</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
       </c>
       <c r="G19" t="s">
         <v>13</v>
@@ -1047,7 +1049,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -1059,10 +1061,10 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
         <v>22</v>
-      </c>
-      <c r="F20" t="s">
-        <v>23</v>
       </c>
       <c r="G20" t="s">
         <v>13</v>
@@ -1076,7 +1078,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -1088,10 +1090,10 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
         <v>22</v>
-      </c>
-      <c r="F21" t="s">
-        <v>23</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -1105,7 +1107,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -1117,10 +1119,10 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
         <v>24</v>
-      </c>
-      <c r="F22" t="s">
-        <v>25</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
@@ -1134,7 +1136,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -1146,10 +1148,10 @@
         <v>11</v>
       </c>
       <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
         <v>24</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
       </c>
       <c r="G23" t="s">
         <v>13</v>
@@ -1163,7 +1165,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -1175,10 +1177,10 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
         <v>24</v>
-      </c>
-      <c r="F24" t="s">
-        <v>25</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>

</xml_diff>